<commit_message>
Added missing album art to Hillsong, S&S. Data cleaning in Hillsong spreadsheet.
</commit_message>
<xml_diff>
--- a/WorshipCreator.TestData/Source/Books/ShaneAndShane/ShaneAndShane.xlsx
+++ b/WorshipCreator.TestData/Source/Books/ShaneAndShane/ShaneAndShane.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PageOptimizer\Data\WorshipCreator.TestData\Source\Books\ShaneAndShane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A0E26F-FE24-4980-9EF3-F60A0EA95230}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB89150-8E7E-4481-9135-AB3C2FE5CEBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18360" yWindow="4485" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{1898BBCD-4A5D-4B3F-9317-061045B18130}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2665" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2673" uniqueCount="773">
   <si>
     <t>G</t>
   </si>
@@ -2535,7 +2535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2586,6 +2586,7 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3294,7 +3295,9 @@
       <c r="J3" s="24" t="s">
         <v>759</v>
       </c>
-      <c r="K3" s="32"/>
+      <c r="K3" s="34" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="B4">
@@ -3322,7 +3325,9 @@
       <c r="J4" s="24" t="s">
         <v>761</v>
       </c>
-      <c r="K4" s="32"/>
+      <c r="K4" s="34" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="5" spans="1:12">
       <c r="B5">
@@ -3350,7 +3355,9 @@
       <c r="J5" s="24" t="s">
         <v>760</v>
       </c>
-      <c r="K5" s="32"/>
+      <c r="K5" s="34" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6">
@@ -3378,7 +3385,9 @@
       <c r="J6" s="24" t="s">
         <v>762</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="34" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7">
@@ -3439,7 +3448,9 @@
       <c r="J8" s="24">
         <v>40120</v>
       </c>
-      <c r="K8" s="32"/>
+      <c r="K8" s="34" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="9" spans="1:12">
       <c r="B9">
@@ -3467,7 +3478,9 @@
       <c r="J9" s="24">
         <v>40470</v>
       </c>
-      <c r="K9" s="32"/>
+      <c r="K9" s="34" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="B10">
@@ -3495,7 +3508,9 @@
       <c r="J10" s="31">
         <v>40820</v>
       </c>
-      <c r="K10" s="33"/>
+      <c r="K10" s="33" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="B11">
@@ -3523,7 +3538,9 @@
       <c r="J11" s="31">
         <v>41408</v>
       </c>
-      <c r="K11" s="33"/>
+      <c r="K11" s="33" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="B12">

</xml_diff>